<commit_message>
feat(CMM): part provider mod hints & cleanups
</commit_message>
<xml_diff>
--- a/CharacterCustomizerPlus/LangMod/CN/cmm_localizations.xlsx
+++ b/CharacterCustomizerPlus/LangMod/CN/cmm_localizations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CharacterCustomizerPlus\LangMod\CN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7854E61D-1672-4D74-B47A-D0829DA16E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0093945-EC61-4A87-9856-E0BF5A3219AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5070" yWindow="3075" windowWidth="25395" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,15 +47,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ccm_ui_remove</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>無し</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>空白</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmm_ui_remove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cmm_ui_unknown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未知Mod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不明なMOD</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -108,13 +120,12 @@
     </font>
     <font>
       <sz val="16"/>
-      <name val="Yu Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
+      <name val="微软雅黑"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -443,7 +454,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -489,16 +500,28 @@
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" ht="23.25" x14ac:dyDescent="0.4">
       <c r="A4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
+    </row>
+    <row r="5" spans="1:4" ht="23.25" x14ac:dyDescent="0.4">
+      <c r="A5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>